<commit_message>
Scrap webpages with Beautiful Soup
</commit_message>
<xml_diff>
--- a/dvf14_chart.xlsx
+++ b/dvf14_chart.xlsx
@@ -135,158 +135,6 @@
     </indexedColors>
   </colors>
 </styleSheet>
-</file>
-
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
-  <style val="13"/>
-  <chart>
-    <title>
-      <tx>
-        <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:t>Scatter Chart</a:t>
-            </a:r>
-          </a:p>
-        </rich>
-      </tx>
-    </title>
-    <plotArea>
-      <scatterChart>
-        <ser>
-          <idx val="0"/>
-          <order val="0"/>
-          <tx>
-            <strRef>
-              <f>'Sheet2'!B1</f>
-            </strRef>
-          </tx>
-          <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-              <a:noFill/>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </spPr>
-          <marker>
-            <symbol val="diamond"/>
-            <spPr>
-              <a:solidFill xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:srgbClr val="0000FF"/>
-              </a:solidFill>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:solidFill>
-                  <a:srgbClr val="0000FF"/>
-                </a:solidFill>
-                <a:prstDash val="solid"/>
-              </a:ln>
-            </spPr>
-          </marker>
-          <xVal>
-            <numRef>
-              <f>'Sheet2'!$A$2:$A$641</f>
-            </numRef>
-          </xVal>
-          <yVal>
-            <numRef>
-              <f>'Sheet2'!$B$2:$B$641</f>
-            </numRef>
-          </yVal>
-        </ser>
-        <axId val="10"/>
-        <axId val="20"/>
-      </scatterChart>
-      <valAx>
-        <axId val="10"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Surface</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="20"/>
-      </valAx>
-      <valAx>
-        <axId val="20"/>
-        <scaling>
-          <orientation val="minMax"/>
-        </scaling>
-        <axPos val="l"/>
-        <majorGridlines/>
-        <title>
-          <tx>
-            <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:t>Price</a:t>
-                </a:r>
-              </a:p>
-            </rich>
-          </tx>
-        </title>
-        <majorTickMark val="none"/>
-        <minorTickMark val="none"/>
-        <crossAx val="10"/>
-      </valAx>
-    </plotArea>
-    <legend>
-      <legendPos val="r"/>
-    </legend>
-    <plotVisOnly val="1"/>
-    <dispBlanksAs val="gap"/>
-  </chart>
-</chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <oneCellAnchor>
-    <from>
-      <col>3</col>
-      <colOff>0</colOff>
-      <row>1</row>
-      <rowOff>0</rowOff>
-    </from>
-    <ext cx="5400000" cy="2700000"/>
-    <graphicFrame>
-      <nvGraphicFramePr>
-        <cNvPr id="1" name="Chart 1"/>
-        <cNvGraphicFramePr/>
-      </nvGraphicFramePr>
-      <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </graphicFrame>
-    <clientData/>
-  </oneCellAnchor>
-</wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -65211,6 +65059,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>